<commit_message>
Changed iterationNo to permutationNo, and renamed eligibility feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>TC ID</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>RM_02</t>
+  </si>
+  <si>
+    <t>PermutationNo</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,11 +126,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -135,6 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +471,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +486,10 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
@@ -481,10 +500,10 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -493,6 +512,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -501,13 +521,13 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="2" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="2"/>
     <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -521,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
feature file format updates
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="3" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
-  <si>
-    <t>TC ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Augustin</t>
   </si>
@@ -37,9 +34,6 @@
     <t>Amy</t>
   </si>
   <si>
-    <t>RM ID</t>
-  </si>
-  <si>
     <t>Scenario Name</t>
   </si>
   <si>
@@ -73,12 +67,6 @@
     <t>This is an Admin user for Eligiblity</t>
   </si>
   <si>
-    <t>IterationNo</t>
-  </si>
-  <si>
-    <t>SkipTest</t>
-  </si>
-  <si>
     <t>Alien</t>
   </si>
   <si>
@@ -94,14 +82,30 @@
     <t>RM_02</t>
   </si>
   <si>
-    <t>PermutationNo</t>
+    <t xml:space="preserve">Available
+</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Test_Script_Id</t>
+  </si>
+  <si>
+    <t>Permutation_Number</t>
+  </si>
+  <si>
+    <t>Skip_Test</t>
+  </si>
+  <si>
+    <t>Feature_Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,16 +113,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -141,11 +165,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -154,6 +187,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,46 +511,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -520,40 +570,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="37" style="2" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
+    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
     <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -567,16 +619,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2">
         <v>74856</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,16 +639,16 @@
         <v>1221</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2">
         <v>88888</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -611,16 +663,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2">
         <v>54321</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -633,37 +685,37 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -677,13 +729,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
         <v>74856</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,13 +749,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2">
         <v>88888</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -717,13 +769,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
         <v>54321</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated with Test track ALM Client
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Augustin</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Feature_Id</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>RM User</t>
   </si>
 </sst>
 </file>
@@ -511,16 +517,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="57.42578125" customWidth="1"/>
@@ -558,6 +564,16 @@
       </c>
       <c r="E2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -570,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1234</v>
+        <v>22302</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -685,7 +701,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1234</v>
+        <v>22302</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Changed the test id to 22746
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Augustin</t>
   </si>
@@ -101,10 +101,16 @@
     <t>Feature_Id</t>
   </si>
   <si>
-    <t>hr</t>
-  </si>
-  <si>
-    <t>RM User</t>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>WHaque@SEMPRANRGU</t>
+  </si>
+  <si>
+    <t>!!Mar1983</t>
+  </si>
+  <si>
+    <t>This is an Admin user for Recruitment</t>
   </si>
 </sst>
 </file>
@@ -148,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,20 +177,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,8 +189,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -517,49 +512,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
@@ -568,17 +563,27 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -586,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,25 +607,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -629,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>22302</v>
+        <v>22746</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -701,7 +706,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,22 +720,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -739,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>22302</v>
+        <v>22746</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Added WorksheetID, added initialze Scenario in BaseStepDefns
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Credentials" sheetId="3" r:id="rId1"/>
     <sheet name="Common" sheetId="1" r:id="rId2"/>
-    <sheet name="RM_01" sheetId="2" r:id="rId3"/>
+    <sheet name="BEN_FTR_001_Utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Augustin</t>
   </si>
@@ -111,13 +111,25 @@
   </si>
   <si>
     <t>This is an Admin user for Recruitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KMizell@SEMPRANRGU </t>
+  </si>
+  <si>
+    <t>ProKarma2018!</t>
+  </si>
+  <si>
+    <t>Recruitment2</t>
+  </si>
+  <si>
+    <t>This is Ken's user for Recruitment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +141,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,10 +198,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -198,8 +219,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,17 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="57.42578125" customWidth="1"/>
   </cols>
@@ -578,12 +599,30 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -592,7 +631,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +745,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
supports Helix test script id, alm properties are configurable in testconfig.properties
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Augustin</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>This is Ken's user for Recruitment</t>
+  </si>
+  <si>
+    <t>Helix_Test_Case_Number</t>
+  </si>
+  <si>
+    <t>BEN_22746</t>
+  </si>
+  <si>
+    <t>BEN_1221</t>
+  </si>
+  <si>
+    <t>BEN_4321</t>
   </si>
 </sst>
 </file>
@@ -537,7 +549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -628,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,13 +653,14 @@
     <col min="1" max="1" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="29.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -656,82 +671,94 @@
         <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>22746</v>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2">
+        <v>22746</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>74856</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2">
         <v>1221</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>88888</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
-        <v>4321</v>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2">
+        <v>4321</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>54321</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -742,23 +769,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="39.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -769,72 +796,84 @@
         <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>22746</v>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="2">
+        <v>22746</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>74856</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>1221</v>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="2">
+        <v>1221</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>88888</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
-        <v>4321</v>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="2">
+        <v>4321</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>54321</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Encrypted username and passwords for test business accounts and alm accounts
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -58,15 +58,6 @@
     <t>UserType</t>
   </si>
   <si>
-    <t>azarate</t>
-  </si>
-  <si>
-    <t>Vantage2018</t>
-  </si>
-  <si>
-    <t>This is an Admin user for Eligiblity</t>
-  </si>
-  <si>
     <t>Alien</t>
   </si>
   <si>
@@ -104,21 +95,6 @@
     <t>Recruitment</t>
   </si>
   <si>
-    <t>WHaque@SEMPRANRGU</t>
-  </si>
-  <si>
-    <t>!!Mar1983</t>
-  </si>
-  <si>
-    <t>This is an Admin user for Recruitment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMizell@SEMPRANRGU </t>
-  </si>
-  <si>
-    <t>ProKarma2018!</t>
-  </si>
-  <si>
     <t>Recruitment2</t>
   </si>
   <si>
@@ -135,13 +111,37 @@
   </si>
   <si>
     <t>BEN_4321</t>
+  </si>
+  <si>
+    <t>C43334ECC030748B9501A9DCDAA87178</t>
+  </si>
+  <si>
+    <t>This is an Admin user for Recruitment-Wasim's id</t>
+  </si>
+  <si>
+    <t>This is an Admin user for Eligiblity-Agustin's id</t>
+  </si>
+  <si>
+    <t>0EE90B7F550DC5BE42CC9C6BA8FBDBB46FCCEF123AF64FAFC7E54185F19D4DE2</t>
+  </si>
+  <si>
+    <t>717CCED269EB1D984F953ECA444840634814CADB4FCDAB7FCB6AC2C17EDC4691</t>
+  </si>
+  <si>
+    <t>624E960DF8B16CF7ED32A425663CD7E2</t>
+  </si>
+  <si>
+    <t>25CED681E01F7023F4AF0D973946802E</t>
+  </si>
+  <si>
+    <t>49BC901F154770AE8B2B510F5158CD68</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,14 +153,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,9 +202,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -231,10 +222,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,7 +540,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +563,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>8</v>
@@ -581,59 +571,59 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" display="WHaque@SEMPRANRGU"/>
+    <hyperlink ref="B4" r:id="rId2" display="KMizell@SEMPRANRGU "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -645,7 +635,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,22 +652,22 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>4</v>
@@ -691,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -703,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2">
         <v>74856</v>
@@ -717,7 +707,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>1221</v>
@@ -726,13 +719,13 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2">
         <v>88888</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -741,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -753,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2">
         <v>54321</v>
@@ -787,16 +780,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -813,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -836,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -851,7 +844,7 @@
         <v>88888</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -859,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
encrypted user credentials in test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Eligibility_TestData.xlsx
+++ b/src/test/resources/testdata/Eligibility_TestData.xlsx
@@ -17,11 +17,6 @@
     <sheet name="BEN_FTR_001_Utilities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -188,16 +183,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,7 +535,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>